<commit_message>
✅ more coverage in excelService
</commit_message>
<xml_diff>
--- a/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelMultipleNwk.xlsx
+++ b/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelMultipleNwk.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.einig\IdeaProjects\Praktikumsplaner\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.nischwitz\Documents\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{563BBC63-8AF8-4908-94B7-043E3E00BD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF760FB-6967-42DD-89CA-EB60309A4657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="-4470" windowWidth="28800" windowHeight="15375" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -94,6 +93,9 @@
   </si>
   <si>
     <t>Do + Fr</t>
+  </si>
+  <si>
+    <t>Mo + Di + Mi + Do + Fr</t>
   </si>
 </sst>
 </file>
@@ -498,19 +500,19 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="2" max="2" width="16.69921875" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.09765625" customWidth="1"/>
-    <col min="5" max="5" width="20.8984375" customWidth="1"/>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -561,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -592,108 +594,108 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>